<commit_message>
for future reference (excel file exact format)
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\PycharmProjects\YucaipaCityPermit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AF5E77-ECD2-466C-B178-5D935810C732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949AC109-6173-4D04-BDF0-328FA47A46E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A73F84BD-3259-49CC-9357-80230FC0B03D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Input</t>
   </si>
@@ -112,22 +112,31 @@
     <t>red = get rid of soon</t>
   </si>
   <si>
-    <t>Free Tag from Salvador (one of them)</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>July 21, 2022</t>
-  </si>
-  <si>
-    <t>20930869AP/CP/BP</t>
-  </si>
-  <si>
-    <t>Holiday</t>
-  </si>
-  <si>
-    <t>34184 County Line Rd, Space #18</t>
+    <t>12821 4th St, Space #20</t>
+  </si>
+  <si>
+    <t>Crestview</t>
+  </si>
+  <si>
+    <t>AAF 5539</t>
+  </si>
+  <si>
+    <t>August 8, 2022</t>
+  </si>
+  <si>
+    <t>manuf_name</t>
+  </si>
+  <si>
+    <t>decal_num</t>
+  </si>
+  <si>
+    <t>yr_of_manuf</t>
+  </si>
+  <si>
+    <t>Hallmark</t>
+  </si>
+  <si>
+    <t>LAT1307</t>
   </si>
 </sst>
 </file>
@@ -243,6 +252,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>199157</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47254</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A1BEFDA-39DD-BEAD-2EBD-EAC5F1FA35E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8181975" y="1647825"/>
+          <a:ext cx="6942857" cy="2971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EEFF51-2E49-41C8-A9EE-073E0BCFAF77}">
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="5"/>
@@ -607,7 +665,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -619,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -648,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="6">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -661,7 +719,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -673,8 +731,8 @@
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
+      <c r="D11" s="4">
+        <v>161983</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -686,11 +744,9 @@
         <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -701,7 +757,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="11">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -714,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="11">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -727,7 +783,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="11">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -740,7 +796,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="11">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -754,7 +810,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -765,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="11">
-        <v>3.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -776,7 +832,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -787,7 +843,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="11">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
@@ -797,9 +853,38 @@
       <c r="B21">
         <v>17</v>
       </c>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>